<commit_message>
edit process blank names
</commit_message>
<xml_diff>
--- a/Raw NPOC Data/20221111_Readme_NPOC_TN_COMPASS_EXCHANGE_WSOC_n10.xlsx
+++ b/Raw NPOC Data/20221111_Readme_NPOC_TN_COMPASS_EXCHANGE_WSOC_n10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/julia_mcelhinny_pnnl_gov/Documents/Documents/GitHub/COMPASS-DOE/JuliaSULI/Raw NPOC Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{0508A712-87D3-544E-8FC4-3EA00EB5B9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C66F52EE-17DA-429B-89D2-75EFC4390DBB}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{0508A712-87D3-544E-8FC4-3EA00EB5B9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CA49A43-7822-4406-A188-7E53E032D47D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{012F814C-8D41-3D47-A566-B7C284ABE7DD}"/>
   </bookViews>
@@ -135,24 +135,6 @@
     <t>Blank5</t>
   </si>
   <si>
-    <t>blank-filter1</t>
-  </si>
-  <si>
-    <t>blank-sol1</t>
-  </si>
-  <si>
-    <t>blank-filter2</t>
-  </si>
-  <si>
-    <t>blank-sol2</t>
-  </si>
-  <si>
-    <t>blank-filter3</t>
-  </si>
-  <si>
-    <t>blank-sol3</t>
-  </si>
-  <si>
     <t>Blank6</t>
   </si>
   <si>
@@ -211,6 +193,24 @@
   </si>
   <si>
     <t>GENERAL NOTE: only NPOC run, TN was good from last run but NPOC had a lot over the 100ppm standard curve, so re-ran with more dilute samples. Cal curve looks good. Blanks a bit high due to high sample concentrations.</t>
+  </si>
+  <si>
+    <t>EC1_blank-filter1</t>
+  </si>
+  <si>
+    <t>EC1_blank-sol1</t>
+  </si>
+  <si>
+    <t>EC1_blank-filter2</t>
+  </si>
+  <si>
+    <t>EC1_blank-sol2</t>
+  </si>
+  <si>
+    <t>EC1_blank-filter3</t>
+  </si>
+  <si>
+    <t>EC1_blank-sol3</t>
   </si>
 </sst>
 </file>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1887ACA-464F-F442-BF69-365F75A60B67}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -678,10 +678,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -692,7 +692,7 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -703,7 +703,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -714,7 +714,7 @@
         <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -835,7 +835,7 @@
         <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -846,7 +846,7 @@
         <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -857,7 +857,7 @@
         <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -868,12 +868,12 @@
         <v>37</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B30">
         <v>38</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B31">
         <v>39</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>40</v>
@@ -906,7 +906,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B33">
         <v>41</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B34">
         <v>42</v>
@@ -928,7 +928,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B35">
         <v>43</v>
@@ -939,57 +939,57 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>